<commit_message>
Dokonceny program kapacitancie a priehyb
</commit_message>
<xml_diff>
--- a/filename1.xlsx
+++ b/filename1.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>ide to</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,170 +348,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
-        <v>-20</v>
-      </c>
-      <c r="B1">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>-19</v>
-      </c>
-      <c r="B2">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>-18</v>
-      </c>
-      <c r="B3">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>-17</v>
-      </c>
-      <c r="B4">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>-16</v>
-      </c>
-      <c r="B5">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>-15</v>
-      </c>
-      <c r="B6">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>-14</v>
-      </c>
-      <c r="B7">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>-13</v>
-      </c>
-      <c r="B8">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>-12</v>
-      </c>
-      <c r="B9">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>-11</v>
-      </c>
-      <c r="B10">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>-10</v>
-      </c>
-      <c r="B11">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>-9</v>
-      </c>
-      <c r="B12">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>-8</v>
-      </c>
-      <c r="B13">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>-7</v>
-      </c>
-      <c r="B14">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>-6</v>
-      </c>
-      <c r="B15">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>-5</v>
-      </c>
-      <c r="B16">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>-4</v>
-      </c>
-      <c r="B17">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>-3</v>
-      </c>
-      <c r="B18">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>-2</v>
-      </c>
-      <c r="B19">
-        <v>0.2563992608768094</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>-1</v>
-      </c>
-      <c r="B20">
-        <v>0.2563992608768094</v>
+    <row r="6" spans="6:6">
+      <c r="F6" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>